<commit_message>
test NetworkTopoNoToolFT fully working; cleaning
</commit_message>
<xml_diff>
--- a/DependencyRule.xlsx
+++ b/DependencyRule.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="29">
   <si>
     <t>&lt;</t>
   </si>
@@ -641,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1066,61 +1066,84 @@
         <v>7</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>0</v>
       </c>
       <c r="F20" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>10</v>
       </c>
-      <c r="B21" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>7</v>
+      <c r="B21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>2</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>10</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" t="s">
+        <v>27</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F22" s="1">
-        <v>1</v>
-      </c>
-      <c r="G22" s="1" t="s">
+      <c r="C23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>